<commit_message>
Atualizando planilha sem filtros
</commit_message>
<xml_diff>
--- a/public/carteira-pedidos.xlsx
+++ b/public/carteira-pedidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pietro\Downloads\pedidos-bamelo\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CF82ECE-ACE0-4849-A9B3-4BDE37A72D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E824A2B-E72A-417B-A257-6400DFA0C94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="857" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="BASE" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE!$A$2:$M$432</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE!$A$2:$M$443</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -2170,14 +2170,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E426117-AF64-47A6-A38A-31ED0921FF70}">
-  <sheetPr codeName="Planilha2" filterMode="1"/>
+  <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:M2987"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="13" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="13" ySplit="2" topLeftCell="N304" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M158" sqref="M158"/>
+      <selection pane="bottomRight" activeCell="M422" sqref="M422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2214,7 +2214,7 @@
       <c r="L1" s="30"/>
       <c r="M1" s="31"/>
     </row>
-    <row r="2" spans="1:13" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>51351</v>
       </c>
@@ -2292,7 +2292,7 @@
       </c>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>51163</v>
       </c>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="M4" s="14"/>
     </row>
-    <row r="5" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>51285</v>
       </c>
@@ -2370,7 +2370,7 @@
       </c>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>51349</v>
       </c>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>51350</v>
       </c>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="M7" s="14"/>
     </row>
-    <row r="8" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>51352</v>
       </c>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>51353</v>
       </c>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="M9" s="14"/>
     </row>
-    <row r="10" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>51354</v>
       </c>
@@ -2555,7 +2555,7 @@
       </c>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>51154</v>
       </c>
@@ -2594,7 +2594,7 @@
       </c>
       <c r="M11" s="14"/>
     </row>
-    <row r="12" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>51156</v>
       </c>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>50982</v>
       </c>
@@ -2670,7 +2670,7 @@
       </c>
       <c r="M13" s="14"/>
     </row>
-    <row r="14" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>51147</v>
       </c>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>51148</v>
       </c>
@@ -2744,7 +2744,7 @@
       </c>
       <c r="M15" s="14"/>
     </row>
-    <row r="16" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>50790</v>
       </c>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>50937</v>
       </c>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="M17" s="14"/>
     </row>
-    <row r="18" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>50870</v>
       </c>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>51263</v>
       </c>
@@ -2900,7 +2900,7 @@
       </c>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>51158</v>
       </c>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="M20" s="14"/>
     </row>
-    <row r="21" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>51264</v>
       </c>
@@ -2978,7 +2978,7 @@
       </c>
       <c r="M21" s="14"/>
     </row>
-    <row r="22" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>51265</v>
       </c>
@@ -3017,7 +3017,7 @@
       </c>
       <c r="M22" s="14"/>
     </row>
-    <row r="23" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>50932</v>
       </c>
@@ -3056,7 +3056,7 @@
       </c>
       <c r="M23" s="14"/>
     </row>
-    <row r="24" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>51259</v>
       </c>
@@ -3095,7 +3095,7 @@
       </c>
       <c r="M24" s="14"/>
     </row>
-    <row r="25" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>51266</v>
       </c>
@@ -3134,7 +3134,7 @@
       </c>
       <c r="M25" s="14"/>
     </row>
-    <row r="26" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>50145</v>
       </c>
@@ -3173,7 +3173,7 @@
       </c>
       <c r="M26" s="14"/>
     </row>
-    <row r="27" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>50743</v>
       </c>
@@ -3212,7 +3212,7 @@
       </c>
       <c r="M27" s="14"/>
     </row>
-    <row r="28" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>50992</v>
       </c>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="M28" s="14"/>
     </row>
-    <row r="29" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>51330</v>
       </c>
@@ -3290,7 +3290,7 @@
       </c>
       <c r="M29" s="14"/>
     </row>
-    <row r="30" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>51260</v>
       </c>
@@ -3329,7 +3329,7 @@
       </c>
       <c r="M30" s="14"/>
     </row>
-    <row r="31" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>51430</v>
       </c>
@@ -3368,7 +3368,7 @@
       </c>
       <c r="M31" s="14"/>
     </row>
-    <row r="32" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>50407</v>
       </c>
@@ -3407,7 +3407,7 @@
       </c>
       <c r="M32" s="14"/>
     </row>
-    <row r="33" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>51433</v>
       </c>
@@ -3444,7 +3444,7 @@
       </c>
       <c r="M33" s="14"/>
     </row>
-    <row r="34" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>50933</v>
       </c>
@@ -3483,7 +3483,7 @@
       </c>
       <c r="M34" s="14"/>
     </row>
-    <row r="35" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>50935</v>
       </c>
@@ -3522,7 +3522,7 @@
       </c>
       <c r="M35" s="14"/>
     </row>
-    <row r="36" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>50938</v>
       </c>
@@ -3561,7 +3561,7 @@
       </c>
       <c r="M36" s="14"/>
     </row>
-    <row r="37" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>51058</v>
       </c>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="M37" s="14"/>
     </row>
-    <row r="38" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>51059</v>
       </c>
@@ -3639,7 +3639,7 @@
       </c>
       <c r="M38" s="14"/>
     </row>
-    <row r="39" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>50934</v>
       </c>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="M39" s="14"/>
     </row>
-    <row r="40" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>51261</v>
       </c>
@@ -3717,7 +3717,7 @@
       </c>
       <c r="M40" s="14"/>
     </row>
-    <row r="41" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>51267</v>
       </c>
@@ -3756,7 +3756,7 @@
       </c>
       <c r="M41" s="14"/>
     </row>
-    <row r="42" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>50936</v>
       </c>
@@ -3795,7 +3795,7 @@
       </c>
       <c r="M42" s="14"/>
     </row>
-    <row r="43" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>51364</v>
       </c>
@@ -3834,7 +3834,7 @@
       </c>
       <c r="M43" s="14"/>
     </row>
-    <row r="44" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>51361</v>
       </c>
@@ -3871,7 +3871,7 @@
       </c>
       <c r="M44" s="14"/>
     </row>
-    <row r="45" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>50939</v>
       </c>
@@ -3910,7 +3910,7 @@
       </c>
       <c r="M45" s="14"/>
     </row>
-    <row r="46" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>51655</v>
       </c>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="M46" s="14"/>
     </row>
-    <row r="47" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>51656</v>
       </c>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="M47" s="14"/>
     </row>
-    <row r="48" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>51657</v>
       </c>
@@ -4027,7 +4027,7 @@
       </c>
       <c r="M48" s="14"/>
     </row>
-    <row r="49" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>51658</v>
       </c>
@@ -4066,7 +4066,7 @@
       </c>
       <c r="M49" s="14"/>
     </row>
-    <row r="50" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>51659</v>
       </c>
@@ -4105,7 +4105,7 @@
       </c>
       <c r="M50" s="14"/>
     </row>
-    <row r="51" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>51660</v>
       </c>
@@ -4144,7 +4144,7 @@
       </c>
       <c r="M51" s="14"/>
     </row>
-    <row r="52" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>51262</v>
       </c>
@@ -4183,7 +4183,7 @@
       </c>
       <c r="M52" s="14"/>
     </row>
-    <row r="53" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>51282</v>
       </c>
@@ -4222,7 +4222,7 @@
       </c>
       <c r="M53" s="14"/>
     </row>
-    <row r="54" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>50278</v>
       </c>
@@ -4261,7 +4261,7 @@
       </c>
       <c r="M54" s="14"/>
     </row>
-    <row r="55" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>51514</v>
       </c>
@@ -4298,7 +4298,7 @@
       </c>
       <c r="M55" s="14"/>
     </row>
-    <row r="56" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>51289</v>
       </c>
@@ -4337,7 +4337,7 @@
       </c>
       <c r="M56" s="14"/>
     </row>
-    <row r="57" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <v>51472</v>
       </c>
@@ -4374,7 +4374,7 @@
       </c>
       <c r="M57" s="14"/>
     </row>
-    <row r="58" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <v>51473</v>
       </c>
@@ -4411,7 +4411,7 @@
       </c>
       <c r="M58" s="14"/>
     </row>
-    <row r="59" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <v>50774</v>
       </c>
@@ -4450,7 +4450,7 @@
       </c>
       <c r="M59" s="14"/>
     </row>
-    <row r="60" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>51283</v>
       </c>
@@ -4489,7 +4489,7 @@
       </c>
       <c r="M60" s="14"/>
     </row>
-    <row r="61" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <v>51475</v>
       </c>
@@ -4526,7 +4526,7 @@
       </c>
       <c r="M61" s="14"/>
     </row>
-    <row r="62" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <v>51476</v>
       </c>
@@ -4563,7 +4563,7 @@
       </c>
       <c r="M62" s="14"/>
     </row>
-    <row r="63" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>51477</v>
       </c>
@@ -4600,7 +4600,7 @@
       </c>
       <c r="M63" s="14"/>
     </row>
-    <row r="64" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>51478</v>
       </c>
@@ -4637,7 +4637,7 @@
       </c>
       <c r="M64" s="14"/>
     </row>
-    <row r="65" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <v>50940</v>
       </c>
@@ -4676,7 +4676,7 @@
       </c>
       <c r="M65" s="14"/>
     </row>
-    <row r="66" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>51284</v>
       </c>
@@ -4715,7 +4715,7 @@
       </c>
       <c r="M66" s="14"/>
     </row>
-    <row r="67" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>51572</v>
       </c>
@@ -4754,7 +4754,7 @@
       </c>
       <c r="M67" s="14"/>
     </row>
-    <row r="68" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>51595</v>
       </c>
@@ -4791,7 +4791,7 @@
       </c>
       <c r="M68" s="14"/>
     </row>
-    <row r="69" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>51584</v>
       </c>
@@ -4828,7 +4828,7 @@
       </c>
       <c r="M69" s="14"/>
     </row>
-    <row r="70" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>51588</v>
       </c>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="M70" s="14"/>
     </row>
-    <row r="71" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>51642</v>
       </c>
@@ -4902,7 +4902,7 @@
       </c>
       <c r="M71" s="14"/>
     </row>
-    <row r="72" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>51643</v>
       </c>
@@ -4939,7 +4939,7 @@
       </c>
       <c r="M72" s="14"/>
     </row>
-    <row r="73" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>51644</v>
       </c>
@@ -4976,7 +4976,7 @@
       </c>
       <c r="M73" s="14"/>
     </row>
-    <row r="74" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <v>51645</v>
       </c>
@@ -5013,7 +5013,7 @@
       </c>
       <c r="M74" s="14"/>
     </row>
-    <row r="75" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>51646</v>
       </c>
@@ -5050,7 +5050,7 @@
       </c>
       <c r="M75" s="14"/>
     </row>
-    <row r="76" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>51647</v>
       </c>
@@ -5087,7 +5087,7 @@
       </c>
       <c r="M76" s="14"/>
     </row>
-    <row r="77" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>51596</v>
       </c>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="M77" s="14"/>
     </row>
-    <row r="78" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>51597</v>
       </c>
@@ -5161,7 +5161,7 @@
       </c>
       <c r="M78" s="14"/>
     </row>
-    <row r="79" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>51157</v>
       </c>
@@ -5200,7 +5200,7 @@
       </c>
       <c r="M79" s="14"/>
     </row>
-    <row r="80" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>50941</v>
       </c>
@@ -5239,7 +5239,7 @@
       </c>
       <c r="M80" s="14"/>
     </row>
-    <row r="81" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>51287</v>
       </c>
@@ -5278,7 +5278,7 @@
       </c>
       <c r="M81" s="14"/>
     </row>
-    <row r="82" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>51164</v>
       </c>
@@ -5317,7 +5317,7 @@
       </c>
       <c r="M82" s="14"/>
     </row>
-    <row r="83" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>51165</v>
       </c>
@@ -5356,7 +5356,7 @@
       </c>
       <c r="M83" s="14"/>
     </row>
-    <row r="84" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>51159</v>
       </c>
@@ -5395,7 +5395,7 @@
       </c>
       <c r="M84" s="14"/>
     </row>
-    <row r="85" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>51609</v>
       </c>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="M85" s="14"/>
     </row>
-    <row r="86" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>51286</v>
       </c>
@@ -5473,7 +5473,7 @@
       </c>
       <c r="M86" s="14"/>
     </row>
-    <row r="87" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>51333</v>
       </c>
@@ -5512,7 +5512,7 @@
       </c>
       <c r="M87" s="14"/>
     </row>
-    <row r="88" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>51670</v>
       </c>
@@ -5549,7 +5549,7 @@
       </c>
       <c r="M88" s="14"/>
     </row>
-    <row r="89" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>51288</v>
       </c>
@@ -5588,7 +5588,7 @@
       </c>
       <c r="M89" s="14"/>
     </row>
-    <row r="90" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>50871</v>
       </c>
@@ -5627,7 +5627,7 @@
       </c>
       <c r="M90" s="14"/>
     </row>
-    <row r="91" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>51568</v>
       </c>
@@ -5666,7 +5666,7 @@
       </c>
       <c r="M91" s="14"/>
     </row>
-    <row r="92" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>52037</v>
       </c>
@@ -5705,7 +5705,7 @@
       </c>
       <c r="M92" s="14"/>
     </row>
-    <row r="93" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>51690</v>
       </c>
@@ -5744,7 +5744,7 @@
       </c>
       <c r="M93" s="14"/>
     </row>
-    <row r="94" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>51139</v>
       </c>
@@ -5783,7 +5783,7 @@
       </c>
       <c r="M94" s="14"/>
     </row>
-    <row r="95" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>51610</v>
       </c>
@@ -5822,7 +5822,7 @@
       </c>
       <c r="M95" s="14"/>
     </row>
-    <row r="96" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>51611</v>
       </c>
@@ -5861,7 +5861,7 @@
       </c>
       <c r="M96" s="14"/>
     </row>
-    <row r="97" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
         <v>51612</v>
       </c>
@@ -5900,7 +5900,7 @@
       </c>
       <c r="M97" s="14"/>
     </row>
-    <row r="98" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <v>51614</v>
       </c>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="M98" s="14"/>
     </row>
-    <row r="99" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <v>51615</v>
       </c>
@@ -5978,7 +5978,7 @@
       </c>
       <c r="M99" s="25"/>
     </row>
-    <row r="100" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>51616</v>
       </c>
@@ -6017,7 +6017,7 @@
       </c>
       <c r="M100" s="25"/>
     </row>
-    <row r="101" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>51618</v>
       </c>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="M101" s="25"/>
     </row>
-    <row r="102" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
         <v>51620</v>
       </c>
@@ -6095,7 +6095,7 @@
       </c>
       <c r="M102" s="25"/>
     </row>
-    <row r="103" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A103" s="9">
         <v>51622</v>
       </c>
@@ -6134,7 +6134,7 @@
       </c>
       <c r="M103" s="25"/>
     </row>
-    <row r="104" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A104" s="9">
         <v>51623</v>
       </c>
@@ -6173,7 +6173,7 @@
       </c>
       <c r="M104" s="25"/>
     </row>
-    <row r="105" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A105" s="9">
         <v>50421</v>
       </c>
@@ -6212,7 +6212,7 @@
       </c>
       <c r="M105" s="25"/>
     </row>
-    <row r="106" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A106" s="9">
         <v>50827</v>
       </c>
@@ -6251,7 +6251,7 @@
       </c>
       <c r="M106" s="25"/>
     </row>
-    <row r="107" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A107" s="9">
         <v>51671</v>
       </c>
@@ -6290,7 +6290,7 @@
       </c>
       <c r="M107" s="25"/>
     </row>
-    <row r="108" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A108" s="9">
         <v>51003</v>
       </c>
@@ -6329,7 +6329,7 @@
       </c>
       <c r="M108" s="25"/>
     </row>
-    <row r="109" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A109" s="9">
         <v>50424</v>
       </c>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="M109" s="14"/>
     </row>
-    <row r="110" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A110" s="9">
         <v>51569</v>
       </c>
@@ -6407,7 +6407,7 @@
       </c>
       <c r="M110" s="25"/>
     </row>
-    <row r="111" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A111" s="9">
         <v>51362</v>
       </c>
@@ -6444,7 +6444,7 @@
       </c>
       <c r="M111" s="25"/>
     </row>
-    <row r="112" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A112" s="9">
         <v>51363</v>
       </c>
@@ -6481,7 +6481,7 @@
       </c>
       <c r="M112" s="25"/>
     </row>
-    <row r="113" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A113" s="9">
         <v>50423</v>
       </c>
@@ -6520,7 +6520,7 @@
       </c>
       <c r="M113" s="25"/>
     </row>
-    <row r="114" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A114" s="9">
         <v>51570</v>
       </c>
@@ -6559,7 +6559,7 @@
       </c>
       <c r="M114" s="25"/>
     </row>
-    <row r="115" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A115" s="9">
         <v>51727</v>
       </c>
@@ -6598,7 +6598,7 @@
       </c>
       <c r="M115" s="25"/>
     </row>
-    <row r="116" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A116" s="9">
         <v>51728</v>
       </c>
@@ -6637,7 +6637,7 @@
       </c>
       <c r="M116" s="25"/>
     </row>
-    <row r="117" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A117" s="9">
         <v>51729</v>
       </c>
@@ -6676,7 +6676,7 @@
       </c>
       <c r="M117" s="25"/>
     </row>
-    <row r="118" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A118" s="9">
         <v>51730</v>
       </c>
@@ -6715,7 +6715,7 @@
       </c>
       <c r="M118" s="25"/>
     </row>
-    <row r="119" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A119" s="9">
         <v>51731</v>
       </c>
@@ -6754,7 +6754,7 @@
       </c>
       <c r="M119" s="25"/>
     </row>
-    <row r="120" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A120" s="9">
         <v>51155</v>
       </c>
@@ -6793,7 +6793,7 @@
       </c>
       <c r="M120" s="25"/>
     </row>
-    <row r="121" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A121" s="9">
         <v>51672</v>
       </c>
@@ -6832,7 +6832,7 @@
       </c>
       <c r="M121" s="14"/>
     </row>
-    <row r="122" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A122" s="9">
         <v>51580</v>
       </c>
@@ -6871,7 +6871,7 @@
       </c>
       <c r="M122" s="25"/>
     </row>
-    <row r="123" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A123" s="9">
         <v>51365</v>
       </c>
@@ -6910,7 +6910,7 @@
       </c>
       <c r="M123" s="25"/>
     </row>
-    <row r="124" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A124" s="9">
         <v>51758</v>
       </c>
@@ -6947,7 +6947,7 @@
       </c>
       <c r="M124" s="14"/>
     </row>
-    <row r="125" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A125" s="9">
         <v>51888</v>
       </c>
@@ -6986,7 +6986,7 @@
       </c>
       <c r="M125" s="14"/>
     </row>
-    <row r="126" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A126" s="9">
         <v>51889</v>
       </c>
@@ -7025,7 +7025,7 @@
       </c>
       <c r="M126" s="14"/>
     </row>
-    <row r="127" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A127" s="9">
         <v>51887</v>
       </c>
@@ -7064,7 +7064,7 @@
       </c>
       <c r="M127" s="14"/>
     </row>
-    <row r="128" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A128" s="9">
         <v>51862</v>
       </c>
@@ -7101,7 +7101,7 @@
       </c>
       <c r="M128" s="14"/>
     </row>
-    <row r="129" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A129" s="9">
         <v>51860</v>
       </c>
@@ -7138,7 +7138,7 @@
       </c>
       <c r="M129" s="14"/>
     </row>
-    <row r="130" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A130" s="9">
         <v>50533</v>
       </c>
@@ -7177,7 +7177,7 @@
       </c>
       <c r="M130" s="14"/>
     </row>
-    <row r="131" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A131" s="9">
         <v>51732</v>
       </c>
@@ -7216,7 +7216,7 @@
       </c>
       <c r="M131" s="14"/>
     </row>
-    <row r="132" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A132" s="9">
         <v>51733</v>
       </c>
@@ -7255,7 +7255,7 @@
       </c>
       <c r="M132" s="14"/>
     </row>
-    <row r="133" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A133" s="9">
         <v>52038</v>
       </c>
@@ -7294,7 +7294,7 @@
       </c>
       <c r="M133" s="14"/>
     </row>
-    <row r="134" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A134" s="9">
         <v>51841</v>
       </c>
@@ -7333,7 +7333,7 @@
       </c>
       <c r="M134" s="14"/>
     </row>
-    <row r="135" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A135" s="9">
         <v>51996</v>
       </c>
@@ -7372,7 +7372,7 @@
       </c>
       <c r="M135" s="14"/>
     </row>
-    <row r="136" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A136" s="9">
         <v>51140</v>
       </c>
@@ -7411,7 +7411,7 @@
       </c>
       <c r="M136" s="14"/>
     </row>
-    <row r="137" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A137" s="9">
         <v>52007</v>
       </c>
@@ -7450,7 +7450,7 @@
       </c>
       <c r="M137" s="14"/>
     </row>
-    <row r="138" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A138" s="9">
         <v>51583</v>
       </c>
@@ -7489,7 +7489,7 @@
       </c>
       <c r="M138" s="14"/>
     </row>
-    <row r="139" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A139" s="9">
         <v>50791</v>
       </c>
@@ -7528,7 +7528,7 @@
       </c>
       <c r="M139" s="14"/>
     </row>
-    <row r="140" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A140" s="9">
         <v>51004</v>
       </c>
@@ -7567,7 +7567,7 @@
       </c>
       <c r="M140" s="25"/>
     </row>
-    <row r="141" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A141" s="9">
         <v>51853</v>
       </c>
@@ -7606,7 +7606,7 @@
       </c>
       <c r="M141" s="14"/>
     </row>
-    <row r="142" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A142" s="9">
         <v>51854</v>
       </c>
@@ -7645,7 +7645,7 @@
       </c>
       <c r="M142" s="14"/>
     </row>
-    <row r="143" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A143" s="9">
         <v>51855</v>
       </c>
@@ -7684,7 +7684,7 @@
       </c>
       <c r="M143" s="14"/>
     </row>
-    <row r="144" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A144" s="9">
         <v>51856</v>
       </c>
@@ -7723,7 +7723,7 @@
       </c>
       <c r="M144" s="14"/>
     </row>
-    <row r="145" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A145" s="9">
         <v>51857</v>
       </c>
@@ -7762,7 +7762,7 @@
       </c>
       <c r="M145" s="14"/>
     </row>
-    <row r="146" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A146" s="9">
         <v>51858</v>
       </c>
@@ -7801,7 +7801,7 @@
       </c>
       <c r="M146" s="14"/>
     </row>
-    <row r="147" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A147" s="9">
         <v>51859</v>
       </c>
@@ -7951,7 +7951,7 @@
       </c>
       <c r="M150" s="14"/>
     </row>
-    <row r="151" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A151" s="9">
         <v>51840</v>
       </c>
@@ -7990,7 +7990,7 @@
       </c>
       <c r="M151" s="14"/>
     </row>
-    <row r="152" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A152" s="9">
         <v>51997</v>
       </c>
@@ -8029,7 +8029,7 @@
       </c>
       <c r="M152" s="14"/>
     </row>
-    <row r="153" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A153" s="9">
         <v>51792</v>
       </c>
@@ -8066,7 +8066,7 @@
       </c>
       <c r="M153" s="14"/>
     </row>
-    <row r="154" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A154" s="9">
         <v>51794</v>
       </c>
@@ -8103,7 +8103,7 @@
       </c>
       <c r="M154" s="14"/>
     </row>
-    <row r="155" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A155" s="9">
         <v>51796</v>
       </c>
@@ -8140,7 +8140,7 @@
       </c>
       <c r="M155" s="14"/>
     </row>
-    <row r="156" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A156" s="9">
         <v>51797</v>
       </c>
@@ -8251,7 +8251,7 @@
       </c>
       <c r="M158" s="14"/>
     </row>
-    <row r="159" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A159" s="9">
         <v>51910</v>
       </c>
@@ -8288,7 +8288,7 @@
       </c>
       <c r="M159" s="14"/>
     </row>
-    <row r="160" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A160" s="9">
         <v>51943</v>
       </c>
@@ -8325,7 +8325,7 @@
       </c>
       <c r="M160" s="14"/>
     </row>
-    <row r="161" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A161" s="9">
         <v>51975</v>
       </c>
@@ -8364,7 +8364,7 @@
       </c>
       <c r="M161" s="14"/>
     </row>
-    <row r="162" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A162" s="9">
         <v>51981</v>
       </c>
@@ -8403,7 +8403,7 @@
       </c>
       <c r="M162" s="14"/>
     </row>
-    <row r="163" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A163" s="9">
         <v>51982</v>
       </c>
@@ -8442,7 +8442,7 @@
       </c>
       <c r="M163" s="14"/>
     </row>
-    <row r="164" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A164" s="9">
         <v>51976</v>
       </c>
@@ -8481,7 +8481,7 @@
       </c>
       <c r="M164" s="14"/>
     </row>
-    <row r="165" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A165" s="9">
         <v>51977</v>
       </c>
@@ -8520,7 +8520,7 @@
       </c>
       <c r="M165" s="14"/>
     </row>
-    <row r="166" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A166" s="9">
         <v>51978</v>
       </c>
@@ -8559,7 +8559,7 @@
       </c>
       <c r="M166" s="14"/>
     </row>
-    <row r="167" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A167" s="9">
         <v>51979</v>
       </c>
@@ -8596,7 +8596,7 @@
       </c>
       <c r="M167" s="14"/>
     </row>
-    <row r="168" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A168" s="9">
         <v>51980</v>
       </c>
@@ -8633,7 +8633,7 @@
       </c>
       <c r="M168" s="14"/>
     </row>
-    <row r="169" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A169" s="9">
         <v>51985</v>
       </c>
@@ -8670,7 +8670,7 @@
       </c>
       <c r="M169" s="14"/>
     </row>
-    <row r="170" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A170" s="9">
         <v>52012</v>
       </c>
@@ -8709,7 +8709,7 @@
       </c>
       <c r="M170" s="14"/>
     </row>
-    <row r="171" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A171" s="9">
         <v>52013</v>
       </c>
@@ -8748,7 +8748,7 @@
       </c>
       <c r="M171" s="14"/>
     </row>
-    <row r="172" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A172" s="9">
         <v>52014</v>
       </c>
@@ -8787,7 +8787,7 @@
       </c>
       <c r="M172" s="14"/>
     </row>
-    <row r="173" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A173" s="9">
         <v>52015</v>
       </c>
@@ -8826,7 +8826,7 @@
       </c>
       <c r="M173" s="14"/>
     </row>
-    <row r="174" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A174" s="9">
         <v>52016</v>
       </c>
@@ -8865,7 +8865,7 @@
       </c>
       <c r="M174" s="14"/>
     </row>
-    <row r="175" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A175" s="9">
         <v>52017</v>
       </c>
@@ -8904,7 +8904,7 @@
       </c>
       <c r="M175" s="14"/>
     </row>
-    <row r="176" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A176" s="9">
         <v>52018</v>
       </c>
@@ -8943,7 +8943,7 @@
       </c>
       <c r="M176" s="14"/>
     </row>
-    <row r="177" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A177" s="9">
         <v>52019</v>
       </c>
@@ -8982,7 +8982,7 @@
       </c>
       <c r="M177" s="14"/>
     </row>
-    <row r="178" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A178" s="9">
         <v>52020</v>
       </c>
@@ -9021,7 +9021,7 @@
       </c>
       <c r="M178" s="14"/>
     </row>
-    <row r="179" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A179" s="9">
         <v>51988</v>
       </c>
@@ -9058,7 +9058,7 @@
       </c>
       <c r="M179" s="14"/>
     </row>
-    <row r="180" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A180" s="9">
         <v>51989</v>
       </c>
@@ -9097,7 +9097,7 @@
         <v>7177.17</v>
       </c>
     </row>
-    <row r="181" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A181" s="9">
         <v>51990</v>
       </c>
@@ -9136,7 +9136,7 @@
       </c>
       <c r="M181" s="14"/>
     </row>
-    <row r="182" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A182" s="9">
         <v>51991</v>
       </c>
@@ -9175,7 +9175,7 @@
       </c>
       <c r="M182" s="14"/>
     </row>
-    <row r="183" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A183" s="9">
         <v>51992</v>
       </c>
@@ -9214,7 +9214,7 @@
       </c>
       <c r="M183" s="14"/>
     </row>
-    <row r="184" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A184" s="9">
         <v>51993</v>
       </c>
@@ -9253,7 +9253,7 @@
       </c>
       <c r="M184" s="14"/>
     </row>
-    <row r="185" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A185" s="9">
         <v>51994</v>
       </c>
@@ -9292,7 +9292,7 @@
       </c>
       <c r="M185" s="14"/>
     </row>
-    <row r="186" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A186" s="9">
         <v>50241</v>
       </c>
@@ -9331,7 +9331,7 @@
       </c>
       <c r="M186" s="14"/>
     </row>
-    <row r="187" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A187" s="9">
         <v>51998</v>
       </c>
@@ -9370,7 +9370,7 @@
       </c>
       <c r="M187" s="14"/>
     </row>
-    <row r="188" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A188" s="9">
         <v>51999</v>
       </c>
@@ -9409,7 +9409,7 @@
       </c>
       <c r="M188" s="14"/>
     </row>
-    <row r="189" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A189" s="9">
         <v>52004</v>
       </c>
@@ -9448,7 +9448,7 @@
       </c>
       <c r="M189" s="14"/>
     </row>
-    <row r="190" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A190" s="9">
         <v>52039</v>
       </c>
@@ -9487,7 +9487,7 @@
       </c>
       <c r="M190" s="14"/>
     </row>
-    <row r="191" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A191" s="9">
         <v>52000</v>
       </c>
@@ -9526,7 +9526,7 @@
       </c>
       <c r="M191" s="14"/>
     </row>
-    <row r="192" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A192" s="9">
         <v>52040</v>
       </c>
@@ -9565,7 +9565,7 @@
       </c>
       <c r="M192" s="14"/>
     </row>
-    <row r="193" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A193" s="9">
         <v>51581</v>
       </c>
@@ -9604,7 +9604,7 @@
       </c>
       <c r="M193" s="25"/>
     </row>
-    <row r="194" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A194" s="9">
         <v>52001</v>
       </c>
@@ -9643,7 +9643,7 @@
       </c>
       <c r="M194" s="14"/>
     </row>
-    <row r="195" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A195" s="9">
         <v>52002</v>
       </c>
@@ -9682,7 +9682,7 @@
       </c>
       <c r="M195" s="14"/>
     </row>
-    <row r="196" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A196" s="9">
         <v>52006</v>
       </c>
@@ -9721,7 +9721,7 @@
       </c>
       <c r="M196" s="14"/>
     </row>
-    <row r="197" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A197" s="9">
         <v>52041</v>
       </c>
@@ -9760,7 +9760,7 @@
       </c>
       <c r="M197" s="14"/>
     </row>
-    <row r="198" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A198" s="9">
         <v>51995</v>
       </c>
@@ -9799,7 +9799,7 @@
       </c>
       <c r="M198" s="14"/>
     </row>
-    <row r="199" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A199" s="9">
         <v>52009</v>
       </c>
@@ -9838,7 +9838,7 @@
       </c>
       <c r="M199" s="14"/>
     </row>
-    <row r="200" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A200" s="9">
         <v>52021</v>
       </c>
@@ -9875,7 +9875,7 @@
       </c>
       <c r="M200" s="14"/>
     </row>
-    <row r="201" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A201" s="9">
         <v>52023</v>
       </c>
@@ -9914,7 +9914,7 @@
       </c>
       <c r="M201" s="14"/>
     </row>
-    <row r="202" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A202" s="9">
         <v>52024</v>
       </c>
@@ -9953,7 +9953,7 @@
       </c>
       <c r="M202" s="14"/>
     </row>
-    <row r="203" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A203" s="9">
         <v>52025</v>
       </c>
@@ -9992,7 +9992,7 @@
       </c>
       <c r="M203" s="14"/>
     </row>
-    <row r="204" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A204" s="9">
         <v>52026</v>
       </c>
@@ -10031,7 +10031,7 @@
       </c>
       <c r="M204" s="14"/>
     </row>
-    <row r="205" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A205" s="9">
         <v>52027</v>
       </c>
@@ -10070,7 +10070,7 @@
       </c>
       <c r="M205" s="14"/>
     </row>
-    <row r="206" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A206" s="9">
         <v>52028</v>
       </c>
@@ -10109,7 +10109,7 @@
       </c>
       <c r="M206" s="14"/>
     </row>
-    <row r="207" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A207" s="9">
         <v>52036</v>
       </c>
@@ -10148,7 +10148,7 @@
       </c>
       <c r="M207" s="14"/>
     </row>
-    <row r="208" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A208" s="9">
         <v>52042</v>
       </c>
@@ -10187,7 +10187,7 @@
       </c>
       <c r="M208" s="14"/>
     </row>
-    <row r="209" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A209" s="9">
         <v>50422</v>
       </c>
@@ -10226,7 +10226,7 @@
       </c>
       <c r="M209" s="14"/>
     </row>
-    <row r="210" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A210" s="9">
         <v>52005</v>
       </c>
@@ -10265,7 +10265,7 @@
       </c>
       <c r="M210" s="14"/>
     </row>
-    <row r="211" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A211" s="9">
         <v>50828</v>
       </c>
@@ -10304,7 +10304,7 @@
       </c>
       <c r="M211" s="14"/>
     </row>
-    <row r="212" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A212" s="9">
         <v>52008</v>
       </c>
@@ -10343,7 +10343,7 @@
       </c>
       <c r="M212" s="14"/>
     </row>
-    <row r="213" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A213" s="9">
         <v>51582</v>
       </c>
@@ -10382,7 +10382,7 @@
       </c>
       <c r="M213" s="14"/>
     </row>
-    <row r="214" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A214" s="9">
         <v>52045</v>
       </c>
@@ -10530,7 +10530,7 @@
       </c>
       <c r="M217" s="14"/>
     </row>
-    <row r="218" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A218" s="9">
         <v>52076</v>
       </c>
@@ -10567,7 +10567,7 @@
       </c>
       <c r="M218" s="27"/>
     </row>
-    <row r="219" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A219" s="9">
         <v>52075</v>
       </c>
@@ -10604,7 +10604,7 @@
       </c>
       <c r="M219" s="14"/>
     </row>
-    <row r="220" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A220" s="9">
         <v>52097</v>
       </c>
@@ -10641,7 +10641,7 @@
       </c>
       <c r="M220" s="14"/>
     </row>
-    <row r="221" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A221" s="9">
         <v>52120</v>
       </c>
@@ -10678,7 +10678,7 @@
       </c>
       <c r="M221" s="14"/>
     </row>
-    <row r="222" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A222" s="9">
         <v>51985</v>
       </c>
@@ -10715,7 +10715,7 @@
       </c>
       <c r="M222" s="14"/>
     </row>
-    <row r="223" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A223" s="9">
         <v>52103</v>
       </c>
@@ -10754,7 +10754,7 @@
       </c>
       <c r="M223" s="14"/>
     </row>
-    <row r="224" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A224" s="9">
         <v>52109</v>
       </c>
@@ -10793,7 +10793,7 @@
       </c>
       <c r="M224" s="14"/>
     </row>
-    <row r="225" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A225" s="9">
         <v>52110</v>
       </c>
@@ -10869,7 +10869,7 @@
       </c>
       <c r="M226" s="14"/>
     </row>
-    <row r="227" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A227" s="9">
         <v>52117</v>
       </c>
@@ -10908,7 +10908,7 @@
         <v>7687.68</v>
       </c>
     </row>
-    <row r="228" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A228" s="9">
         <v>52116</v>
       </c>
@@ -10947,7 +10947,7 @@
         <v>7631.12</v>
       </c>
     </row>
-    <row r="229" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A229" s="9">
         <v>52162</v>
       </c>
@@ -10984,7 +10984,7 @@
       </c>
       <c r="M229" s="14"/>
     </row>
-    <row r="230" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A230" s="9">
         <v>52163</v>
       </c>
@@ -11021,7 +11021,7 @@
       </c>
       <c r="M230" s="14"/>
     </row>
-    <row r="231" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A231" s="9">
         <v>52164</v>
       </c>
@@ -11058,7 +11058,7 @@
       </c>
       <c r="M231" s="14"/>
     </row>
-    <row r="232" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A232" s="9">
         <v>52161</v>
       </c>
@@ -11095,7 +11095,7 @@
       </c>
       <c r="M232" s="14"/>
     </row>
-    <row r="233" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A233" s="9">
         <v>52146</v>
       </c>
@@ -11132,7 +11132,7 @@
       </c>
       <c r="M233" s="14"/>
     </row>
-    <row r="234" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A234" s="9">
         <v>52225</v>
       </c>
@@ -11169,7 +11169,7 @@
       </c>
       <c r="M234" s="27"/>
     </row>
-    <row r="235" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A235" s="9">
         <v>52226</v>
       </c>
@@ -11206,7 +11206,7 @@
       </c>
       <c r="M235" s="27"/>
     </row>
-    <row r="236" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A236" s="9">
         <v>52227</v>
       </c>
@@ -11245,7 +11245,7 @@
         <v>3930.71</v>
       </c>
     </row>
-    <row r="237" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A237" s="9">
         <v>52246</v>
       </c>
@@ -11284,7 +11284,7 @@
       </c>
       <c r="M237" s="14"/>
     </row>
-    <row r="238" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A238" s="9">
         <v>52253</v>
       </c>
@@ -11323,7 +11323,7 @@
       </c>
       <c r="M238" s="14"/>
     </row>
-    <row r="239" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A239" s="9">
         <v>52254</v>
       </c>
@@ -11361,7 +11361,7 @@
       </c>
       <c r="M239" s="27"/>
     </row>
-    <row r="240" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A240" s="9">
         <v>52284</v>
       </c>
@@ -11402,7 +11402,7 @@
       </c>
       <c r="M240" s="27"/>
     </row>
-    <row r="241" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A241" s="9">
         <v>52285</v>
       </c>
@@ -11443,7 +11443,7 @@
       </c>
       <c r="M241" s="27"/>
     </row>
-    <row r="242" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A242" s="9">
         <v>52286</v>
       </c>
@@ -11484,7 +11484,7 @@
       </c>
       <c r="M242" s="27"/>
     </row>
-    <row r="243" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A243" s="9">
         <v>52287</v>
       </c>
@@ -11525,7 +11525,7 @@
       </c>
       <c r="M243" s="27"/>
     </row>
-    <row r="244" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A244" s="9">
         <v>52288</v>
       </c>
@@ -11566,7 +11566,7 @@
       </c>
       <c r="M244" s="27"/>
     </row>
-    <row r="245" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A245" s="9">
         <v>52305</v>
       </c>
@@ -11609,7 +11609,7 @@
       </c>
       <c r="M245" s="14"/>
     </row>
-    <row r="246" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A246" s="9">
         <v>52337</v>
       </c>
@@ -11650,7 +11650,7 @@
       </c>
       <c r="M246" s="27"/>
     </row>
-    <row r="247" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A247" s="9">
         <v>52338</v>
       </c>
@@ -11691,7 +11691,7 @@
       </c>
       <c r="M247" s="27"/>
     </row>
-    <row r="248" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A248" s="9">
         <v>52351</v>
       </c>
@@ -11734,7 +11734,7 @@
       </c>
       <c r="M248" s="27"/>
     </row>
-    <row r="249" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A249" s="9">
         <v>52352</v>
       </c>
@@ -11777,7 +11777,7 @@
       </c>
       <c r="M249" s="27"/>
     </row>
-    <row r="250" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A250" s="9">
         <v>52353</v>
       </c>
@@ -11820,7 +11820,7 @@
       </c>
       <c r="M250" s="27"/>
     </row>
-    <row r="251" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A251" s="9" t="s">
         <v>397</v>
       </c>
@@ -11863,7 +11863,7 @@
       </c>
       <c r="M251" s="27"/>
     </row>
-    <row r="252" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A252" s="9">
         <v>52370</v>
       </c>
@@ -11906,7 +11906,7 @@
       </c>
       <c r="M252" s="27"/>
     </row>
-    <row r="253" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A253" s="9">
         <v>52360</v>
       </c>
@@ -11947,7 +11947,7 @@
       </c>
       <c r="M253" s="27"/>
     </row>
-    <row r="254" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A254" s="9">
         <v>52361</v>
       </c>
@@ -11988,7 +11988,7 @@
       </c>
       <c r="M254" s="27"/>
     </row>
-    <row r="255" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A255" s="9">
         <v>52362</v>
       </c>
@@ -12234,7 +12234,7 @@
       </c>
       <c r="M260" s="27"/>
     </row>
-    <row r="261" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A261" s="9">
         <v>52379</v>
       </c>
@@ -12277,7 +12277,7 @@
       </c>
       <c r="M261" s="27"/>
     </row>
-    <row r="262" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A262" s="9">
         <v>52380</v>
       </c>
@@ -12320,7 +12320,7 @@
       </c>
       <c r="M262" s="27"/>
     </row>
-    <row r="263" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A263" s="9">
         <v>52381</v>
       </c>
@@ -12363,7 +12363,7 @@
       </c>
       <c r="M263" s="27"/>
     </row>
-    <row r="264" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A264" s="9">
         <v>52406</v>
       </c>
@@ -12406,7 +12406,7 @@
       </c>
       <c r="M264" s="27"/>
     </row>
-    <row r="265" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A265" s="9">
         <v>52407</v>
       </c>
@@ -12449,7 +12449,7 @@
       </c>
       <c r="M265" s="27"/>
     </row>
-    <row r="266" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A266" s="9">
         <v>52408</v>
       </c>
@@ -12492,7 +12492,7 @@
       </c>
       <c r="M266" s="27"/>
     </row>
-    <row r="267" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A267" s="9">
         <v>52409</v>
       </c>
@@ -12535,7 +12535,7 @@
       </c>
       <c r="M267" s="27"/>
     </row>
-    <row r="268" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A268" s="9">
         <v>52410</v>
       </c>
@@ -12578,7 +12578,7 @@
       </c>
       <c r="M268" s="27"/>
     </row>
-    <row r="269" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A269" s="9">
         <v>52429</v>
       </c>
@@ -12616,7 +12616,7 @@
       </c>
       <c r="M269" s="27"/>
     </row>
-    <row r="270" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A270" s="9">
         <v>52437</v>
       </c>
@@ -12657,7 +12657,7 @@
       </c>
       <c r="M270" s="27"/>
     </row>
-    <row r="271" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A271" s="9">
         <v>52463</v>
       </c>
@@ -12698,7 +12698,7 @@
       </c>
       <c r="M271" s="27"/>
     </row>
-    <row r="272" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A272" s="9">
         <v>52464</v>
       </c>
@@ -12739,7 +12739,7 @@
       </c>
       <c r="M272" s="27"/>
     </row>
-    <row r="273" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A273" s="9">
         <v>52465</v>
       </c>
@@ -12780,7 +12780,7 @@
       </c>
       <c r="M273" s="27"/>
     </row>
-    <row r="274" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A274" s="9">
         <v>52466</v>
       </c>
@@ -12821,7 +12821,7 @@
       </c>
       <c r="M274" s="27"/>
     </row>
-    <row r="275" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A275" s="9">
         <v>52503</v>
       </c>
@@ -13067,7 +13067,7 @@
       </c>
       <c r="M280" s="27"/>
     </row>
-    <row r="281" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A281" s="9">
         <v>52582</v>
       </c>
@@ -13108,7 +13108,7 @@
       </c>
       <c r="M281" s="27"/>
     </row>
-    <row r="282" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A282" s="9">
         <v>52583</v>
       </c>
@@ -13149,7 +13149,7 @@
       </c>
       <c r="M282" s="27"/>
     </row>
-    <row r="283" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A283" s="9">
         <v>52584</v>
       </c>
@@ -13190,7 +13190,7 @@
       </c>
       <c r="M283" s="27"/>
     </row>
-    <row r="284" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A284" s="9">
         <v>52574</v>
       </c>
@@ -13231,7 +13231,7 @@
       </c>
       <c r="M284" s="27"/>
     </row>
-    <row r="285" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A285" s="9">
         <v>52575</v>
       </c>
@@ -13272,7 +13272,7 @@
       </c>
       <c r="M285" s="27"/>
     </row>
-    <row r="286" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A286" s="9">
         <v>52576</v>
       </c>
@@ -13313,7 +13313,7 @@
       </c>
       <c r="M286" s="27"/>
     </row>
-    <row r="287" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A287" s="9">
         <v>52577</v>
       </c>
@@ -13354,7 +13354,7 @@
       </c>
       <c r="M287" s="27"/>
     </row>
-    <row r="288" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A288" s="9">
         <v>52578</v>
       </c>
@@ -13395,7 +13395,7 @@
       </c>
       <c r="M288" s="27"/>
     </row>
-    <row r="289" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A289" s="9">
         <v>52579</v>
       </c>
@@ -13436,7 +13436,7 @@
       </c>
       <c r="M289" s="27"/>
     </row>
-    <row r="290" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A290" s="9">
         <v>52580</v>
       </c>
@@ -13477,7 +13477,7 @@
       </c>
       <c r="M290" s="27"/>
     </row>
-    <row r="291" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A291" s="9">
         <v>52581</v>
       </c>
@@ -13518,7 +13518,7 @@
       </c>
       <c r="M291" s="27"/>
     </row>
-    <row r="292" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A292" s="9">
         <v>52572</v>
       </c>
@@ -13559,7 +13559,7 @@
       </c>
       <c r="M292" s="27"/>
     </row>
-    <row r="293" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A293" s="9">
         <v>52573</v>
       </c>
@@ -13600,7 +13600,7 @@
       </c>
       <c r="M293" s="27"/>
     </row>
-    <row r="294" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A294" s="9">
         <v>52600</v>
       </c>
@@ -13641,7 +13641,7 @@
       </c>
       <c r="M294" s="27"/>
     </row>
-    <row r="295" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A295" s="9">
         <v>52601</v>
       </c>
@@ -13682,7 +13682,7 @@
       </c>
       <c r="M295" s="27"/>
     </row>
-    <row r="296" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A296" s="9">
         <v>52602</v>
       </c>
@@ -13723,7 +13723,7 @@
       </c>
       <c r="M296" s="27"/>
     </row>
-    <row r="297" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A297" s="9">
         <v>52603</v>
       </c>
@@ -13764,7 +13764,7 @@
       </c>
       <c r="M297" s="27"/>
     </row>
-    <row r="298" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A298" s="9">
         <v>52609</v>
       </c>
@@ -13807,7 +13807,7 @@
       </c>
       <c r="M298" s="27"/>
     </row>
-    <row r="299" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A299" s="9">
         <v>52604</v>
       </c>
@@ -13850,7 +13850,7 @@
       </c>
       <c r="M299" s="27"/>
     </row>
-    <row r="300" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A300" s="9">
         <v>52605</v>
       </c>
@@ -13893,7 +13893,7 @@
       </c>
       <c r="M300" s="27"/>
     </row>
-    <row r="301" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A301" s="9">
         <v>52606</v>
       </c>
@@ -13936,7 +13936,7 @@
       </c>
       <c r="M301" s="27"/>
     </row>
-    <row r="302" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A302" s="9">
         <v>52607</v>
       </c>
@@ -13979,7 +13979,7 @@
       </c>
       <c r="M302" s="27"/>
     </row>
-    <row r="303" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A303" s="9">
         <v>52608</v>
       </c>
@@ -14022,7 +14022,7 @@
       </c>
       <c r="M303" s="27"/>
     </row>
-    <row r="304" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A304" s="9">
         <v>52620</v>
       </c>
@@ -14063,7 +14063,7 @@
       </c>
       <c r="M304" s="27"/>
     </row>
-    <row r="305" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A305" s="9">
         <v>52636</v>
       </c>
@@ -14104,7 +14104,7 @@
       </c>
       <c r="M305" s="27"/>
     </row>
-    <row r="306" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A306" s="9">
         <v>52637</v>
       </c>
@@ -14145,7 +14145,7 @@
       </c>
       <c r="M306" s="27"/>
     </row>
-    <row r="307" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A307" s="9">
         <v>52642</v>
       </c>
@@ -14186,7 +14186,7 @@
       </c>
       <c r="M307" s="27"/>
     </row>
-    <row r="308" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A308" s="9">
         <v>52646</v>
       </c>
@@ -14227,7 +14227,7 @@
       </c>
       <c r="M308" s="27"/>
     </row>
-    <row r="309" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A309" s="9">
         <v>52643</v>
       </c>
@@ -14268,7 +14268,7 @@
       </c>
       <c r="M309" s="27"/>
     </row>
-    <row r="310" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A310" s="9">
         <v>52644</v>
       </c>
@@ -14308,7 +14308,7 @@
       </c>
       <c r="M310" s="27"/>
     </row>
-    <row r="311" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A311" s="9">
         <v>52638</v>
       </c>
@@ -14349,7 +14349,7 @@
       </c>
       <c r="M311" s="27"/>
     </row>
-    <row r="312" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A312" s="9">
         <v>52656</v>
       </c>
@@ -14636,7 +14636,7 @@
       </c>
       <c r="M318" s="27"/>
     </row>
-    <row r="319" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A319" s="9">
         <v>51701</v>
       </c>
@@ -14677,7 +14677,7 @@
       </c>
       <c r="M319" s="27"/>
     </row>
-    <row r="320" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A320" s="9">
         <v>52717</v>
       </c>
@@ -14720,7 +14720,7 @@
       </c>
       <c r="M320" s="27"/>
     </row>
-    <row r="321" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A321" s="9">
         <v>52718</v>
       </c>
@@ -14763,7 +14763,7 @@
       </c>
       <c r="M321" s="27"/>
     </row>
-    <row r="322" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A322" s="9">
         <v>52724</v>
       </c>
@@ -14806,7 +14806,7 @@
       </c>
       <c r="M322" s="27"/>
     </row>
-    <row r="323" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A323" s="9">
         <v>52725</v>
       </c>
@@ -14849,7 +14849,7 @@
       </c>
       <c r="M323" s="27"/>
     </row>
-    <row r="324" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A324" s="9">
         <v>52726</v>
       </c>
@@ -14892,7 +14892,7 @@
       </c>
       <c r="M324" s="27"/>
     </row>
-    <row r="325" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A325" s="9">
         <v>52757</v>
       </c>
@@ -14933,7 +14933,7 @@
       </c>
       <c r="M325" s="27"/>
     </row>
-    <row r="326" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A326" s="9">
         <v>52758</v>
       </c>
@@ -14974,7 +14974,7 @@
       </c>
       <c r="M326" s="27"/>
     </row>
-    <row r="327" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A327" s="9">
         <v>52759</v>
       </c>
@@ -15017,7 +15017,7 @@
       </c>
       <c r="M327" s="27"/>
     </row>
-    <row r="328" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A328" s="9">
         <v>52862</v>
       </c>
@@ -15060,7 +15060,7 @@
       </c>
       <c r="M328" s="27"/>
     </row>
-    <row r="329" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A329" s="9">
         <v>52863</v>
       </c>
@@ -15103,7 +15103,7 @@
       </c>
       <c r="M329" s="27"/>
     </row>
-    <row r="330" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A330" s="9">
         <v>52864</v>
       </c>
@@ -15146,7 +15146,7 @@
       </c>
       <c r="M330" s="27"/>
     </row>
-    <row r="331" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A331" s="9">
         <v>52865</v>
       </c>
@@ -15189,7 +15189,7 @@
       </c>
       <c r="M331" s="27"/>
     </row>
-    <row r="332" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A332" s="9">
         <v>52866</v>
       </c>
@@ -15232,7 +15232,7 @@
       </c>
       <c r="M332" s="27"/>
     </row>
-    <row r="333" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A333" s="9">
         <v>52867</v>
       </c>
@@ -15275,7 +15275,7 @@
       </c>
       <c r="M333" s="27"/>
     </row>
-    <row r="334" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A334" s="9">
         <v>52868</v>
       </c>
@@ -15318,7 +15318,7 @@
       </c>
       <c r="M334" s="27"/>
     </row>
-    <row r="335" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A335" s="9">
         <v>52869</v>
       </c>
@@ -15361,7 +15361,7 @@
       </c>
       <c r="M335" s="27"/>
     </row>
-    <row r="336" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A336" s="9">
         <v>53102</v>
       </c>
@@ -15403,7 +15403,7 @@
       </c>
       <c r="M336" s="27"/>
     </row>
-    <row r="337" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A337" s="9">
         <v>52870</v>
       </c>
@@ -15446,7 +15446,7 @@
       </c>
       <c r="M337" s="27"/>
     </row>
-    <row r="338" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A338" s="9">
         <v>52877</v>
       </c>
@@ -15487,7 +15487,7 @@
       </c>
       <c r="M338" s="27"/>
     </row>
-    <row r="339" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A339" s="9">
         <v>52887</v>
       </c>
@@ -15530,7 +15530,7 @@
       </c>
       <c r="M339" s="27"/>
     </row>
-    <row r="340" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A340" s="9">
         <v>52888</v>
       </c>
@@ -15573,7 +15573,7 @@
       </c>
       <c r="M340" s="27"/>
     </row>
-    <row r="341" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A341" s="9">
         <v>52889</v>
       </c>
@@ -15616,7 +15616,7 @@
       </c>
       <c r="M341" s="27"/>
     </row>
-    <row r="342" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A342" s="9">
         <v>52890</v>
       </c>
@@ -15659,7 +15659,7 @@
       </c>
       <c r="M342" s="27"/>
     </row>
-    <row r="343" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A343" s="9">
         <v>52903</v>
       </c>
@@ -15700,7 +15700,7 @@
       </c>
       <c r="M343" s="27"/>
     </row>
-    <row r="344" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A344" s="9">
         <v>52937</v>
       </c>
@@ -15741,7 +15741,7 @@
       </c>
       <c r="M344" s="27"/>
     </row>
-    <row r="345" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A345" s="9">
         <v>52935</v>
       </c>
@@ -15784,7 +15784,7 @@
       </c>
       <c r="M345" s="27"/>
     </row>
-    <row r="346" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A346" s="9">
         <v>52936</v>
       </c>
@@ -15827,7 +15827,7 @@
       </c>
       <c r="M346" s="27"/>
     </row>
-    <row r="347" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A347" s="9">
         <v>52939</v>
       </c>
@@ -15868,7 +15868,7 @@
       </c>
       <c r="M347" s="27"/>
     </row>
-    <row r="348" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A348" s="9">
         <v>52962</v>
       </c>
@@ -15907,7 +15907,7 @@
       </c>
       <c r="M348" s="27"/>
     </row>
-    <row r="349" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A349" s="9">
         <v>52995</v>
       </c>
@@ -15947,7 +15947,7 @@
       </c>
       <c r="M349" s="27"/>
     </row>
-    <row r="350" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A350" s="9">
         <v>53013</v>
       </c>
@@ -15988,7 +15988,7 @@
       </c>
       <c r="M350" s="27"/>
     </row>
-    <row r="351" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A351" s="9">
         <v>53073</v>
       </c>
@@ -16030,7 +16030,7 @@
       </c>
       <c r="M351" s="27"/>
     </row>
-    <row r="352" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A352" s="9">
         <v>53074</v>
       </c>
@@ -16071,7 +16071,7 @@
       </c>
       <c r="M352" s="27"/>
     </row>
-    <row r="353" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A353" s="9">
         <v>53075</v>
       </c>
@@ -16112,7 +16112,7 @@
       </c>
       <c r="M353" s="27"/>
     </row>
-    <row r="354" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A354" s="9">
         <v>53103</v>
       </c>
@@ -16154,7 +16154,7 @@
       </c>
       <c r="M354" s="27"/>
     </row>
-    <row r="355" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A355" s="9">
         <v>52871</v>
       </c>
@@ -16197,7 +16197,7 @@
       </c>
       <c r="M355" s="27"/>
     </row>
-    <row r="356" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A356" s="9">
         <v>53104</v>
       </c>
@@ -16239,7 +16239,7 @@
       </c>
       <c r="M356" s="27"/>
     </row>
-    <row r="357" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A357" s="9">
         <v>53105</v>
       </c>
@@ -16281,7 +16281,7 @@
       </c>
       <c r="M357" s="27"/>
     </row>
-    <row r="358" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A358" s="9">
         <v>53106</v>
       </c>
@@ -16323,7 +16323,7 @@
       </c>
       <c r="M358" s="27"/>
     </row>
-    <row r="359" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A359" s="9">
         <v>53107</v>
       </c>
@@ -16365,7 +16365,7 @@
       </c>
       <c r="M359" s="27"/>
     </row>
-    <row r="360" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A360" s="9">
         <v>53108</v>
       </c>
@@ -16407,7 +16407,7 @@
       </c>
       <c r="M360" s="27"/>
     </row>
-    <row r="361" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A361" s="9">
         <v>53109</v>
       </c>
@@ -16449,7 +16449,7 @@
       </c>
       <c r="M361" s="27"/>
     </row>
-    <row r="362" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A362" s="9">
         <v>53110</v>
       </c>
@@ -16491,7 +16491,7 @@
       </c>
       <c r="M362" s="27"/>
     </row>
-    <row r="363" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A363" s="9">
         <v>53111</v>
       </c>
@@ -16533,7 +16533,7 @@
       </c>
       <c r="M363" s="27"/>
     </row>
-    <row r="364" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A364" s="9">
         <v>53112</v>
       </c>
@@ -16575,7 +16575,7 @@
       </c>
       <c r="M364" s="27"/>
     </row>
-    <row r="365" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A365" s="9">
         <v>53113</v>
       </c>
@@ -16617,7 +16617,7 @@
       </c>
       <c r="M365" s="27"/>
     </row>
-    <row r="366" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A366" s="9">
         <v>53114</v>
       </c>
@@ -16660,7 +16660,7 @@
       </c>
       <c r="M366" s="27"/>
     </row>
-    <row r="367" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A367" s="9">
         <v>53115</v>
       </c>
@@ -16703,7 +16703,7 @@
       </c>
       <c r="M367" s="27"/>
     </row>
-    <row r="368" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A368" s="9">
         <v>53135</v>
       </c>
@@ -16744,7 +16744,7 @@
       </c>
       <c r="M368" s="27"/>
     </row>
-    <row r="369" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A369" s="9">
         <v>53122</v>
       </c>
@@ -16785,7 +16785,7 @@
       </c>
       <c r="M369" s="27"/>
     </row>
-    <row r="370" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A370" s="9">
         <v>53123</v>
       </c>
@@ -16826,7 +16826,7 @@
       </c>
       <c r="M370" s="27"/>
     </row>
-    <row r="371" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A371" s="9">
         <v>53124</v>
       </c>
@@ -16867,7 +16867,7 @@
       </c>
       <c r="M371" s="27"/>
     </row>
-    <row r="372" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A372" s="9">
         <v>53147</v>
       </c>
@@ -16908,7 +16908,7 @@
       </c>
       <c r="M372" s="27"/>
     </row>
-    <row r="373" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A373" s="9">
         <v>53148</v>
       </c>
@@ -16949,7 +16949,7 @@
       </c>
       <c r="M373" s="27"/>
     </row>
-    <row r="374" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A374" s="9">
         <v>53149</v>
       </c>
@@ -16990,7 +16990,7 @@
       </c>
       <c r="M374" s="27"/>
     </row>
-    <row r="375" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A375" s="9">
         <v>53150</v>
       </c>
@@ -17031,7 +17031,7 @@
       </c>
       <c r="M375" s="27"/>
     </row>
-    <row r="376" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A376" s="9">
         <v>53157</v>
       </c>
@@ -17072,7 +17072,7 @@
       </c>
       <c r="M376" s="27"/>
     </row>
-    <row r="377" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A377" s="9">
         <v>53158</v>
       </c>
@@ -17113,7 +17113,7 @@
       </c>
       <c r="M377" s="27"/>
     </row>
-    <row r="378" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A378" s="9">
         <v>53159</v>
       </c>
@@ -17154,7 +17154,7 @@
       </c>
       <c r="M378" s="27"/>
     </row>
-    <row r="379" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A379" s="9">
         <v>53184</v>
       </c>
@@ -17195,7 +17195,7 @@
       </c>
       <c r="M379" s="27"/>
     </row>
-    <row r="380" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A380" s="9">
         <v>53185</v>
       </c>
@@ -17236,7 +17236,7 @@
       </c>
       <c r="M380" s="27"/>
     </row>
-    <row r="381" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A381" s="9">
         <v>53217</v>
       </c>
@@ -17277,7 +17277,7 @@
       </c>
       <c r="M381" s="27"/>
     </row>
-    <row r="382" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A382" s="9">
         <v>53235</v>
       </c>
@@ -17318,7 +17318,7 @@
       </c>
       <c r="M382" s="27"/>
     </row>
-    <row r="383" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A383" s="9">
         <v>53236</v>
       </c>
@@ -17523,7 +17523,7 @@
       </c>
       <c r="M387" s="27"/>
     </row>
-    <row r="388" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A388" s="9">
         <v>53239</v>
       </c>
@@ -17566,7 +17566,7 @@
       </c>
       <c r="M388" s="27"/>
     </row>
-    <row r="389" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A389" s="9">
         <v>53240</v>
       </c>
@@ -17609,7 +17609,7 @@
       </c>
       <c r="M389" s="27"/>
     </row>
-    <row r="390" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A390" s="9">
         <v>53241</v>
       </c>
@@ -17652,7 +17652,7 @@
       </c>
       <c r="M390" s="27"/>
     </row>
-    <row r="391" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A391" s="9">
         <v>53242</v>
       </c>
@@ -17695,7 +17695,7 @@
       </c>
       <c r="M391" s="27"/>
     </row>
-    <row r="392" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A392" s="9">
         <v>53243</v>
       </c>
@@ -17738,7 +17738,7 @@
       </c>
       <c r="M392" s="27"/>
     </row>
-    <row r="393" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A393" s="9">
         <v>53244</v>
       </c>
@@ -17781,7 +17781,7 @@
       </c>
       <c r="M393" s="27"/>
     </row>
-    <row r="394" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A394" s="9">
         <v>53245</v>
       </c>
@@ -17824,7 +17824,7 @@
       </c>
       <c r="M394" s="27"/>
     </row>
-    <row r="395" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A395" s="9">
         <v>53246</v>
       </c>
@@ -17867,7 +17867,7 @@
       </c>
       <c r="M395" s="27"/>
     </row>
-    <row r="396" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A396" s="9">
         <v>53247</v>
       </c>
@@ -17910,7 +17910,7 @@
       </c>
       <c r="M396" s="27"/>
     </row>
-    <row r="397" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A397" s="9">
         <v>53248</v>
       </c>
@@ -17952,7 +17952,7 @@
       </c>
       <c r="M397" s="27"/>
     </row>
-    <row r="398" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A398" s="9">
         <v>53249</v>
       </c>
@@ -17995,7 +17995,7 @@
       </c>
       <c r="M398" s="27"/>
     </row>
-    <row r="399" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A399" s="9">
         <v>53250</v>
       </c>
@@ -18038,7 +18038,7 @@
       </c>
       <c r="M399" s="27"/>
     </row>
-    <row r="400" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A400" s="9">
         <v>53251</v>
       </c>
@@ -18081,7 +18081,7 @@
       </c>
       <c r="M400" s="27"/>
     </row>
-    <row r="401" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A401" s="9">
         <v>53255</v>
       </c>
@@ -18124,7 +18124,7 @@
       </c>
       <c r="M401" s="27"/>
     </row>
-    <row r="402" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A402" s="9">
         <v>53254</v>
       </c>
@@ -18210,7 +18210,7 @@
       </c>
       <c r="M403" s="27"/>
     </row>
-    <row r="404" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A404" s="9">
         <v>53301</v>
       </c>
@@ -18253,7 +18253,7 @@
       </c>
       <c r="M404" s="27"/>
     </row>
-    <row r="405" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A405" s="9">
         <v>53302</v>
       </c>
@@ -18296,7 +18296,7 @@
       </c>
       <c r="M405" s="27"/>
     </row>
-    <row r="406" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A406" s="9">
         <v>53303</v>
       </c>
@@ -18339,7 +18339,7 @@
       </c>
       <c r="M406" s="27"/>
     </row>
-    <row r="407" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A407" s="9">
         <v>53328</v>
       </c>
@@ -18380,7 +18380,7 @@
       </c>
       <c r="M407" s="27"/>
     </row>
-    <row r="408" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A408" s="9">
         <v>53331</v>
       </c>
@@ -18421,7 +18421,7 @@
       </c>
       <c r="M408" s="27"/>
     </row>
-    <row r="409" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A409" s="9">
         <v>53332</v>
       </c>
@@ -18462,7 +18462,7 @@
       </c>
       <c r="M409" s="27"/>
     </row>
-    <row r="410" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A410" s="9">
         <v>53344</v>
       </c>
@@ -18503,7 +18503,7 @@
       </c>
       <c r="M410" s="27"/>
     </row>
-    <row r="411" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A411" s="9">
         <v>53348</v>
       </c>
@@ -18546,7 +18546,7 @@
       </c>
       <c r="M411" s="27"/>
     </row>
-    <row r="412" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A412" s="9">
         <v>53349</v>
       </c>
@@ -18589,7 +18589,7 @@
       </c>
       <c r="M412" s="27"/>
     </row>
-    <row r="413" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A413" s="9">
         <v>53350</v>
       </c>
@@ -18632,7 +18632,7 @@
       </c>
       <c r="M413" s="27"/>
     </row>
-    <row r="414" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A414" s="9">
         <v>53351</v>
       </c>
@@ -18675,7 +18675,7 @@
       </c>
       <c r="M414" s="27"/>
     </row>
-    <row r="415" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A415" s="9">
         <v>53358</v>
       </c>
@@ -18718,7 +18718,7 @@
       </c>
       <c r="M415" s="27"/>
     </row>
-    <row r="416" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A416" s="9">
         <v>53359</v>
       </c>
@@ -18761,7 +18761,7 @@
       </c>
       <c r="M416" s="27"/>
     </row>
-    <row r="417" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A417" s="9">
         <v>53356</v>
       </c>
@@ -18804,7 +18804,7 @@
       </c>
       <c r="M417" s="27"/>
     </row>
-    <row r="418" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A418" s="9">
         <v>53357</v>
       </c>
@@ -18847,7 +18847,7 @@
       </c>
       <c r="M418" s="27"/>
     </row>
-    <row r="419" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A419" s="9">
         <v>53352</v>
       </c>
@@ -18890,7 +18890,7 @@
       </c>
       <c r="M419" s="27"/>
     </row>
-    <row r="420" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A420" s="9">
         <v>53353</v>
       </c>
@@ -18933,7 +18933,7 @@
       </c>
       <c r="M420" s="27"/>
     </row>
-    <row r="421" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A421" s="9">
         <v>53354</v>
       </c>
@@ -18976,7 +18976,7 @@
       </c>
       <c r="M421" s="27"/>
     </row>
-    <row r="422" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A422" s="9">
         <v>53355</v>
       </c>
@@ -19019,7 +19019,7 @@
       </c>
       <c r="M422" s="27"/>
     </row>
-    <row r="423" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A423" s="9">
         <v>53404</v>
       </c>
@@ -19060,7 +19060,7 @@
       </c>
       <c r="M423" s="27"/>
     </row>
-    <row r="424" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A424" s="9">
         <v>53405</v>
       </c>
@@ -19101,7 +19101,7 @@
       </c>
       <c r="M424" s="27"/>
     </row>
-    <row r="425" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A425" s="9">
         <v>53406</v>
       </c>
@@ -19142,7 +19142,7 @@
       </c>
       <c r="M425" s="27"/>
     </row>
-    <row r="426" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A426" s="9">
         <v>53403</v>
       </c>
@@ -19183,7 +19183,7 @@
       </c>
       <c r="M426" s="27"/>
     </row>
-    <row r="427" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A427" s="9">
         <v>53414</v>
       </c>
@@ -19224,7 +19224,7 @@
       </c>
       <c r="M427" s="27"/>
     </row>
-    <row r="428" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A428" s="9">
         <v>53415</v>
       </c>
@@ -19347,7 +19347,7 @@
       </c>
       <c r="M430" s="27"/>
     </row>
-    <row r="431" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A431" s="9">
         <v>53438</v>
       </c>
@@ -19388,7 +19388,7 @@
       </c>
       <c r="M431" s="27"/>
     </row>
-    <row r="432" spans="1:13" ht="13.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A432" s="9">
         <v>53439</v>
       </c>
@@ -58040,16 +58040,6 @@
       <c r="M2987" s="27"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:M432" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="PINCEIS ROMA"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A335:M365">
-      <sortCondition ref="F2:F400"/>
-    </sortState>
-  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:M1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Substituindo planilha por versão limpa e corrigida
</commit_message>
<xml_diff>
--- a/public/carteira-pedidos.xlsx
+++ b/public/carteira-pedidos.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pietro\Downloads\pedidos-bamelo\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{334697F4-26C4-4B36-ADE8-C99F8B2A4B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D773736C-324C-483B-9B79-BCC548153D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2F5B8E63-56BF-4E60-97C4-BEB94866A626}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{07BA02B7-0E84-48C0-BD94-DA1E37F73FBE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="BASE" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2095,27 +2095,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE29368-B3FD-4841-A45D-17BAA32C9743}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECD9115-4A1E-4C88-BA67-812EC8961755}">
   <dimension ref="A1:M442"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
     <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="12" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>